<commit_message>
Add uploading animation on upload-excel page
</commit_message>
<xml_diff>
--- a/f-end/public/assets/article-excel-template.xlsx
+++ b/f-end/public/assets/article-excel-template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Desktop\New folder\tech-dose\f-end\public\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\tech-dose\f-end\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{662C3774-9E9E-48E9-8EF3-0528BDD11599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25520B51-7F40-45FD-ABDA-5A49F1BBA2D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,27 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>title</t>
   </si>
   <si>
     <t>description</t>
-  </si>
-  <si>
-    <t>thumbnail</t>
-  </si>
-  <si>
-    <t>slug</t>
-  </si>
-  <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>author</t>
   </si>
 </sst>
 </file>
@@ -414,35 +399,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>